<commit_message>
feat: new final map
</commit_message>
<xml_diff>
--- a/Reference/reference.xlsx
+++ b/Reference/reference.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\常嘉硕\大学\中南大学\Games Programming\Pygame\TowerDesign\Reference\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB7FF037-197B-4125-9296-E55CA089DAD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A880557-CA8D-4BE0-B52B-CEF51F335CAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3950" yWindow="2530" windowWidth="19200" windowHeight="12710" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1520" yWindow="1520" windowWidth="19200" windowHeight="11220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Author</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -56,6 +56,18 @@
   </si>
   <si>
     <t>https://opengameart.org/content/rpg-town-pixel-art-assets</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ChatGPT 4o</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pixel Dirt Path</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NULL</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -405,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -446,6 +458,20 @@
         <v>7</v>
       </c>
     </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>

</xml_diff>